<commit_message>
HTGC and TICC code and output finalized
</commit_message>
<xml_diff>
--- a/TICC/all_filings.xlsx
+++ b/TICC/all_filings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanuthuppan/Downloads/**RA Finance**/sec-scraper/TICC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanuthuppan/Downloads/RA/BDC Cleaning/sec-scraper/TICC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3B26A7-F345-CB43-BFA1-00ADD3848E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D45747D-6DD9-2D49-A31B-48865BF7C455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="16960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="57">
   <si>
     <t>Form type</t>
   </si>
@@ -188,13 +188,16 @@
   </si>
   <si>
     <t>https://www.sec.gov/Archives/edgar/data/1259429/000114420414029445/v377449_10q.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1259429/000121390024068478/ea0210294-01_10q.htm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -209,6 +212,11 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -234,11 +242,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -574,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -606,55 +616,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
-        <v>45415</v>
-      </c>
-      <c r="D2" s="2">
-        <v>45382</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
+      <c r="C2" s="5">
+        <v>45518</v>
+      </c>
+      <c r="D2" s="5">
+        <v>45473</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
-        <v>45370</v>
+        <v>45415</v>
       </c>
       <c r="D3" s="2">
-        <v>45291</v>
+        <v>45382</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
-        <v>45238</v>
+        <v>45370</v>
       </c>
       <c r="D4" s="2">
-        <v>45199</v>
+        <v>45291</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -665,13 +675,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="2">
-        <v>45148</v>
+        <v>45238</v>
       </c>
       <c r="D5" s="2">
-        <v>45107</v>
+        <v>45199</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -682,47 +692,47 @@
         <v>6</v>
       </c>
       <c r="C6" s="2">
-        <v>45048</v>
+        <v>45148</v>
       </c>
       <c r="D6" s="2">
-        <v>45016</v>
+        <v>45107</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>45008</v>
+        <v>45048</v>
       </c>
       <c r="D7" s="2">
-        <v>44926</v>
+        <v>45016</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2">
-        <v>44873</v>
+        <v>45008</v>
       </c>
       <c r="D8" s="2">
-        <v>44834</v>
+        <v>44926</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -733,13 +743,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="2">
-        <v>44770</v>
+        <v>44873</v>
       </c>
       <c r="D9" s="2">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -750,47 +760,47 @@
         <v>6</v>
       </c>
       <c r="C10" s="2">
-        <v>44679</v>
+        <v>44770</v>
       </c>
       <c r="D10" s="2">
-        <v>44651</v>
+        <v>44742</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2">
-        <v>44627</v>
+        <v>44679</v>
       </c>
       <c r="D11" s="2">
-        <v>44561</v>
+        <v>44651</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2">
-        <v>44497</v>
+        <v>44627</v>
       </c>
       <c r="D12" s="2">
-        <v>44469</v>
+        <v>44561</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -801,13 +811,13 @@
         <v>6</v>
       </c>
       <c r="C13" s="2">
-        <v>44406</v>
+        <v>44497</v>
       </c>
       <c r="D13" s="2">
-        <v>44377</v>
+        <v>44469</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -818,47 +828,47 @@
         <v>6</v>
       </c>
       <c r="C14" s="2">
-        <v>44315</v>
+        <v>44406</v>
       </c>
       <c r="D14" s="2">
-        <v>44286</v>
+        <v>44377</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2">
-        <v>44277</v>
+        <v>44315</v>
       </c>
       <c r="D15" s="2">
-        <v>44196</v>
+        <v>44286</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2">
-        <v>44132</v>
+        <v>44277</v>
       </c>
       <c r="D16" s="2">
-        <v>44104</v>
+        <v>44196</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -869,13 +879,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="2">
-        <v>44041</v>
+        <v>44132</v>
       </c>
       <c r="D17" s="2">
-        <v>44012</v>
+        <v>44104</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -886,64 +896,64 @@
         <v>6</v>
       </c>
       <c r="C18" s="2">
-        <v>43950</v>
+        <v>44041</v>
       </c>
       <c r="D18" s="2">
-        <v>43921</v>
+        <v>44012</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C19" s="2">
-        <v>43887</v>
+        <v>43950</v>
       </c>
       <c r="D19" s="2">
-        <v>43830</v>
+        <v>43921</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C20" s="2">
-        <v>43770</v>
+        <v>43887</v>
       </c>
       <c r="D20" s="2">
-        <v>43738</v>
+        <v>43830</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C21" s="2">
-        <v>43768</v>
+        <v>43770</v>
       </c>
       <c r="D21" s="2">
         <v>43738</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -954,13 +964,13 @@
         <v>6</v>
       </c>
       <c r="C22" s="2">
-        <v>43677</v>
+        <v>43768</v>
       </c>
       <c r="D22" s="2">
-        <v>43646</v>
+        <v>43738</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -971,47 +981,47 @@
         <v>6</v>
       </c>
       <c r="C23" s="2">
-        <v>43586</v>
+        <v>43677</v>
       </c>
       <c r="D23" s="2">
-        <v>43555</v>
+        <v>43646</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C24" s="2">
-        <v>43524</v>
+        <v>43586</v>
       </c>
       <c r="D24" s="2">
-        <v>43465</v>
+        <v>43555</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C25" s="2">
-        <v>43404</v>
+        <v>43524</v>
       </c>
       <c r="D25" s="2">
-        <v>43373</v>
+        <v>43465</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1022,13 +1032,13 @@
         <v>6</v>
       </c>
       <c r="C26" s="2">
-        <v>43313</v>
+        <v>43404</v>
       </c>
       <c r="D26" s="2">
-        <v>43281</v>
+        <v>43373</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1039,64 +1049,64 @@
         <v>6</v>
       </c>
       <c r="C27" s="2">
-        <v>43222</v>
+        <v>43313</v>
       </c>
       <c r="D27" s="2">
-        <v>43190</v>
+        <v>43281</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C28" s="2">
-        <v>43168</v>
+        <v>43222</v>
       </c>
       <c r="D28" s="2">
-        <v>43100</v>
+        <v>43190</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C29" s="2">
-        <v>43160</v>
+        <v>43168</v>
       </c>
       <c r="D29" s="2">
         <v>43100</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C30" s="2">
-        <v>43041</v>
+        <v>43160</v>
       </c>
       <c r="D30" s="2">
-        <v>43008</v>
+        <v>43100</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1107,13 +1117,13 @@
         <v>6</v>
       </c>
       <c r="C31" s="2">
-        <v>42955</v>
+        <v>43041</v>
       </c>
       <c r="D31" s="2">
-        <v>42916</v>
+        <v>43008</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1124,47 +1134,47 @@
         <v>6</v>
       </c>
       <c r="C32" s="2">
-        <v>42863</v>
+        <v>42955</v>
       </c>
       <c r="D32" s="2">
-        <v>42825</v>
+        <v>42916</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C33" s="2">
-        <v>42797</v>
+        <v>42863</v>
       </c>
       <c r="D33" s="2">
-        <v>42735</v>
+        <v>42825</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C34" s="2">
-        <v>42681</v>
+        <v>42797</v>
       </c>
       <c r="D34" s="2">
-        <v>42643</v>
+        <v>42735</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1175,13 +1185,13 @@
         <v>6</v>
       </c>
       <c r="C35" s="2">
-        <v>42587</v>
+        <v>42681</v>
       </c>
       <c r="D35" s="2">
-        <v>42551</v>
+        <v>42643</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1192,47 +1202,47 @@
         <v>6</v>
       </c>
       <c r="C36" s="2">
-        <v>42495</v>
+        <v>42587</v>
       </c>
       <c r="D36" s="2">
-        <v>42460</v>
+        <v>42551</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C37" s="2">
-        <v>42439</v>
+        <v>42495</v>
       </c>
       <c r="D37" s="2">
-        <v>42369</v>
+        <v>42460</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C38" s="2">
-        <v>42317</v>
+        <v>42439</v>
       </c>
       <c r="D38" s="2">
-        <v>42277</v>
+        <v>42369</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1243,13 +1253,13 @@
         <v>6</v>
       </c>
       <c r="C39" s="2">
-        <v>42223</v>
+        <v>42317</v>
       </c>
       <c r="D39" s="2">
-        <v>42185</v>
+        <v>42277</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1260,47 +1270,47 @@
         <v>6</v>
       </c>
       <c r="C40" s="2">
-        <v>42135</v>
+        <v>42223</v>
       </c>
       <c r="D40" s="2">
-        <v>42094</v>
+        <v>42185</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C41" s="2">
-        <v>42067</v>
+        <v>42135</v>
       </c>
       <c r="D41" s="2">
-        <v>42004</v>
+        <v>42094</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C42" s="2">
-        <v>41949</v>
+        <v>42067</v>
       </c>
       <c r="D42" s="2">
-        <v>41912</v>
+        <v>42004</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1311,13 +1321,13 @@
         <v>6</v>
       </c>
       <c r="C43" s="2">
-        <v>41859</v>
+        <v>41949</v>
       </c>
       <c r="D43" s="2">
-        <v>41820</v>
+        <v>41912</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1328,675 +1338,253 @@
         <v>6</v>
       </c>
       <c r="C44" s="2">
-        <v>41771</v>
+        <v>41859</v>
       </c>
       <c r="D44" s="2">
-        <v>41729</v>
+        <v>41820</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C45" s="2">
-        <v>41715</v>
+        <v>41771</v>
       </c>
       <c r="D45" s="2">
-        <v>41639</v>
+        <v>41729</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="2">
-        <v>41590</v>
-      </c>
-      <c r="D46" s="2">
-        <v>41547</v>
-      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="2">
-        <v>41494</v>
-      </c>
-      <c r="D47" s="2">
-        <v>41455</v>
-      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="2">
-        <v>41403</v>
-      </c>
-      <c r="D48" s="2">
-        <v>41364</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="2">
-        <v>41346</v>
-      </c>
-      <c r="D49" s="2">
-        <v>41274</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="2">
-        <v>41222</v>
-      </c>
-      <c r="D50" s="2">
-        <v>41182</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="2">
-        <v>41124</v>
-      </c>
-      <c r="D51" s="2">
-        <v>41090</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="2">
-        <v>41039</v>
-      </c>
-      <c r="D52" s="2">
-        <v>40999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>7</v>
-      </c>
-      <c r="B53" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="2">
-        <v>40983</v>
-      </c>
-      <c r="D53" s="2">
-        <v>40908</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54" s="2">
-        <v>40856</v>
-      </c>
-      <c r="D54" s="2">
-        <v>40816</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>5</v>
-      </c>
-      <c r="B55" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" s="2">
-        <v>40760</v>
-      </c>
-      <c r="D55" s="2">
-        <v>40724</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="2">
-        <v>40672</v>
-      </c>
-      <c r="D56" s="2">
-        <v>40633</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>7</v>
-      </c>
-      <c r="B57" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" s="2">
-        <v>40611</v>
-      </c>
-      <c r="D57" s="2">
-        <v>40543</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" s="2">
-        <v>40487</v>
-      </c>
-      <c r="D58" s="2">
-        <v>40451</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59" t="s">
-        <v>6</v>
-      </c>
-      <c r="C59" s="2">
-        <v>40396</v>
-      </c>
-      <c r="D59" s="2">
-        <v>40359</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="2">
-        <v>40305</v>
-      </c>
-      <c r="D60" s="2">
-        <v>40268</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>7</v>
-      </c>
-      <c r="B61" t="s">
-        <v>8</v>
-      </c>
-      <c r="C61" s="2">
-        <v>40252</v>
-      </c>
-      <c r="D61" s="2">
-        <v>40178</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62" s="2">
-        <v>40126</v>
-      </c>
-      <c r="D62" s="2">
-        <v>40086</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63" t="s">
-        <v>6</v>
-      </c>
-      <c r="C63" s="2">
-        <v>40035</v>
-      </c>
-      <c r="D63" s="2">
-        <v>39994</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" s="2">
-        <v>39941</v>
-      </c>
-      <c r="D64" s="2">
-        <v>39903</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>7</v>
-      </c>
-      <c r="B65" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="2">
-        <v>39888</v>
-      </c>
-      <c r="D65" s="2">
-        <v>39813</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>5</v>
-      </c>
-      <c r="B66" t="s">
-        <v>6</v>
-      </c>
-      <c r="C66" s="2">
-        <v>39762</v>
-      </c>
-      <c r="D66" s="2">
-        <v>39721</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>5</v>
-      </c>
-      <c r="B67" t="s">
-        <v>6</v>
-      </c>
-      <c r="C67" s="2">
-        <v>39671</v>
-      </c>
-      <c r="D67" s="2">
-        <v>39629</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>5</v>
-      </c>
-      <c r="B68" t="s">
-        <v>6</v>
-      </c>
-      <c r="C68" s="2">
-        <v>39576</v>
-      </c>
-      <c r="D68" s="2">
-        <v>39538</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>7</v>
-      </c>
-      <c r="B69" t="s">
-        <v>8</v>
-      </c>
-      <c r="C69" s="2">
-        <v>39524</v>
-      </c>
-      <c r="D69" s="2">
-        <v>39447</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>5</v>
-      </c>
-      <c r="B70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C70" s="2">
-        <v>39394</v>
-      </c>
-      <c r="D70" s="2">
-        <v>39355</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>5</v>
-      </c>
-      <c r="B71" t="s">
-        <v>6</v>
-      </c>
-      <c r="C71" s="2">
-        <v>39302</v>
-      </c>
-      <c r="D71" s="2">
-        <v>39263</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>5</v>
-      </c>
-      <c r="B72" t="s">
-        <v>6</v>
-      </c>
-      <c r="C72" s="2">
-        <v>39211</v>
-      </c>
-      <c r="D72" s="2">
-        <v>39172</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>11</v>
-      </c>
-      <c r="B73" t="s">
-        <v>12</v>
-      </c>
-      <c r="C73" s="2">
-        <v>39156</v>
-      </c>
-      <c r="D73" s="2">
-        <v>39082</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>7</v>
-      </c>
-      <c r="B74" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" s="2">
-        <v>39154</v>
-      </c>
-      <c r="D74" s="2">
-        <v>39082</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>5</v>
-      </c>
-      <c r="B75" t="s">
-        <v>6</v>
-      </c>
-      <c r="C75" s="2">
-        <v>39030</v>
-      </c>
-      <c r="D75" s="2">
-        <v>38990</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>5</v>
-      </c>
-      <c r="B76" t="s">
-        <v>6</v>
-      </c>
-      <c r="C76" s="2">
-        <v>38938</v>
-      </c>
-      <c r="D76" s="2">
-        <v>38898</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>5</v>
-      </c>
-      <c r="B77" t="s">
-        <v>6</v>
-      </c>
-      <c r="C77" s="2">
-        <v>38846</v>
-      </c>
-      <c r="D77" s="2">
-        <v>38807</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>11</v>
-      </c>
-      <c r="B78" t="s">
-        <v>12</v>
-      </c>
-      <c r="C78" s="2">
-        <v>38821</v>
-      </c>
-      <c r="D78" s="2">
-        <v>38717</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>7</v>
-      </c>
-      <c r="B79" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" s="2">
-        <v>38790</v>
-      </c>
-      <c r="D79" s="2">
-        <v>38717</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>5</v>
-      </c>
-      <c r="B80" t="s">
-        <v>6</v>
-      </c>
-      <c r="C80" s="2">
-        <v>38660</v>
-      </c>
-      <c r="D80" s="2">
-        <v>38625</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" s="2">
-        <v>38572</v>
-      </c>
-      <c r="D81" s="2">
-        <v>38533</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>5</v>
-      </c>
-      <c r="B82" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" s="2">
-        <v>38481</v>
-      </c>
-      <c r="D82" s="2">
-        <v>38442</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>7</v>
-      </c>
-      <c r="B83" t="s">
-        <v>8</v>
-      </c>
-      <c r="C83" s="2">
-        <v>38427</v>
-      </c>
-      <c r="D83" s="2">
-        <v>38352</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>5</v>
-      </c>
-      <c r="B84" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84" s="2">
-        <v>38303</v>
-      </c>
-      <c r="D84" s="2">
-        <v>38260</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>5</v>
-      </c>
-      <c r="B85" t="s">
-        <v>6</v>
-      </c>
-      <c r="C85" s="2">
-        <v>38209</v>
-      </c>
-      <c r="D85" s="2">
-        <v>38168</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>5</v>
-      </c>
-      <c r="B86" t="s">
-        <v>6</v>
-      </c>
-      <c r="C86" s="2">
-        <v>38121</v>
-      </c>
-      <c r="D86" s="2">
-        <v>38077</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>11</v>
-      </c>
-      <c r="B87" t="s">
-        <v>12</v>
-      </c>
-      <c r="C87" s="2">
-        <v>38106</v>
-      </c>
-      <c r="D87" s="2">
-        <v>37986</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>7</v>
-      </c>
-      <c r="B88" t="s">
-        <v>8</v>
-      </c>
-      <c r="C88" s="2">
-        <v>38058</v>
-      </c>
-      <c r="D88" s="2">
-        <v>37986</v>
-      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{3323FF35-F960-2242-917D-11FCC3425EEB}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{78B7B9D1-3198-A942-AB7E-5472A8EDB601}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{6EEA49E0-8CFF-8D44-BA51-ADFA6A0849BB}"/>
-    <hyperlink ref="E6" r:id="rId4" xr:uid="{90DA084D-4133-184D-8C95-F39FB9EF3226}"/>
-    <hyperlink ref="E7" r:id="rId5" xr:uid="{66684A0E-12D9-514C-8864-B0D474A57870}"/>
-    <hyperlink ref="E8" r:id="rId6" xr:uid="{9E6B1AC8-DAD3-264E-BAD2-77A3648A35E4}"/>
-    <hyperlink ref="E9" r:id="rId7" xr:uid="{FF30F675-1982-FD4C-AF45-E502AA400130}"/>
-    <hyperlink ref="E10" r:id="rId8" xr:uid="{401F7663-83E9-AF45-B843-59E40EBF0C7D}"/>
-    <hyperlink ref="E11" r:id="rId9" xr:uid="{972E95F8-B4E4-BA4B-B438-F788F42BCEE6}"/>
-    <hyperlink ref="E12" r:id="rId10" xr:uid="{FECCB3D3-C866-9D48-9500-DC8CC57A6427}"/>
-    <hyperlink ref="E13" r:id="rId11" xr:uid="{B04C8197-66F0-E048-A259-B209AEBDA653}"/>
-    <hyperlink ref="E14" r:id="rId12" xr:uid="{0B691CDF-40A9-BA4A-9414-07C441F17D78}"/>
-    <hyperlink ref="E15" r:id="rId13" xr:uid="{6ADDA0CE-0603-9E48-904C-DF191E111A3A}"/>
-    <hyperlink ref="E16" r:id="rId14" xr:uid="{69FFF26D-BD07-F042-80F7-624227C5406F}"/>
-    <hyperlink ref="E17" r:id="rId15" xr:uid="{BBF43883-C187-6A46-8D00-F3F08FD7EF78}"/>
-    <hyperlink ref="E18" r:id="rId16" xr:uid="{FAD827AA-C1FB-F34F-B951-7A613279A382}"/>
-    <hyperlink ref="E19" r:id="rId17" xr:uid="{2D2FC6BA-A23B-F047-9BFC-C4F6AB2A68FA}"/>
-    <hyperlink ref="E20" r:id="rId18" xr:uid="{91DC0849-A771-2B4D-8789-A3192EE6CCFF}"/>
-    <hyperlink ref="E21" r:id="rId19" xr:uid="{DCC3D403-80C5-5E49-A2EC-ECF64C647897}"/>
-    <hyperlink ref="E22" r:id="rId20" xr:uid="{EB48910F-CAED-4241-8797-59C9BA8AED93}"/>
-    <hyperlink ref="E23" r:id="rId21" xr:uid="{01534F59-E8D4-A541-B4DB-E4E6FDE7D2A7}"/>
-    <hyperlink ref="E24" r:id="rId22" xr:uid="{C2314C5D-0EE5-1244-8978-6CE7B18811FE}"/>
-    <hyperlink ref="E25" r:id="rId23" xr:uid="{6A2887EF-8B3A-0D44-A624-1078642D44C4}"/>
-    <hyperlink ref="E26" r:id="rId24" xr:uid="{9C80C4A9-D364-B447-9AAB-563D067F5FA8}"/>
-    <hyperlink ref="E27" r:id="rId25" xr:uid="{287A05EC-4791-7C4B-AFB2-EF7F9E98085F}"/>
-    <hyperlink ref="E28" r:id="rId26" xr:uid="{C39F56A0-BABE-4748-B88E-1F9C1CD5399C}"/>
-    <hyperlink ref="E29" r:id="rId27" xr:uid="{CD3500D6-E89A-4443-86B3-93668D92BD4C}"/>
-    <hyperlink ref="E30" r:id="rId28" xr:uid="{4E9031F0-8477-664F-B92D-F40965307973}"/>
-    <hyperlink ref="E31" r:id="rId29" location="tCI" xr:uid="{022F7D3A-5030-454F-969D-9C782EBCAE5D}"/>
-    <hyperlink ref="E32" r:id="rId30" location="t2CO" xr:uid="{C04AE7AD-6C42-7C4E-AA71-5AA56D31D27B}"/>
-    <hyperlink ref="E33" r:id="rId31" xr:uid="{8E40C015-C2DE-414B-AA80-95431D3A7B21}"/>
-    <hyperlink ref="E34" r:id="rId32" xr:uid="{46DA0A8F-7FE4-9242-B8D2-37F0D4DE5614}"/>
-    <hyperlink ref="E35" r:id="rId33" xr:uid="{BA2EA337-4B15-6E43-B69B-4DB9C3CC27F9}"/>
-    <hyperlink ref="E36" r:id="rId34" xr:uid="{2B632F1D-0A51-064B-A6DE-8C7259DDAAA9}"/>
-    <hyperlink ref="E37" r:id="rId35" xr:uid="{93B3DFB5-17A9-3243-BD65-EC69EA51348B}"/>
-    <hyperlink ref="E38" r:id="rId36" xr:uid="{A2C45F4E-4F2E-F547-8BC2-3DDF02AC0857}"/>
-    <hyperlink ref="E39" r:id="rId37" xr:uid="{3ABE88F8-913E-6C43-A8C5-978FBBD474BD}"/>
-    <hyperlink ref="E40" r:id="rId38" xr:uid="{9A8E5A03-D834-3D42-89F8-16C00EDC990A}"/>
-    <hyperlink ref="E41" r:id="rId39" xr:uid="{FDB9A909-7A83-1049-B137-579966521ACD}"/>
-    <hyperlink ref="E42" r:id="rId40" xr:uid="{1D912449-03D0-DC44-95AE-E65D2E7E3025}"/>
-    <hyperlink ref="E43" r:id="rId41" xr:uid="{00A22981-CD0A-3D4C-932C-B8AF0DA63F33}"/>
-    <hyperlink ref="E44" r:id="rId42" xr:uid="{2C7CDF4C-39FB-FE44-89A0-C187A8729B6B}"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{3323FF35-F960-2242-917D-11FCC3425EEB}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{78B7B9D1-3198-A942-AB7E-5472A8EDB601}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{6EEA49E0-8CFF-8D44-BA51-ADFA6A0849BB}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{90DA084D-4133-184D-8C95-F39FB9EF3226}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{66684A0E-12D9-514C-8864-B0D474A57870}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{9E6B1AC8-DAD3-264E-BAD2-77A3648A35E4}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{FF30F675-1982-FD4C-AF45-E502AA400130}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{401F7663-83E9-AF45-B843-59E40EBF0C7D}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{972E95F8-B4E4-BA4B-B438-F788F42BCEE6}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{FECCB3D3-C866-9D48-9500-DC8CC57A6427}"/>
+    <hyperlink ref="E14" r:id="rId11" xr:uid="{B04C8197-66F0-E048-A259-B209AEBDA653}"/>
+    <hyperlink ref="E15" r:id="rId12" xr:uid="{0B691CDF-40A9-BA4A-9414-07C441F17D78}"/>
+    <hyperlink ref="E16" r:id="rId13" xr:uid="{6ADDA0CE-0603-9E48-904C-DF191E111A3A}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{69FFF26D-BD07-F042-80F7-624227C5406F}"/>
+    <hyperlink ref="E18" r:id="rId15" xr:uid="{BBF43883-C187-6A46-8D00-F3F08FD7EF78}"/>
+    <hyperlink ref="E19" r:id="rId16" xr:uid="{FAD827AA-C1FB-F34F-B951-7A613279A382}"/>
+    <hyperlink ref="E20" r:id="rId17" xr:uid="{2D2FC6BA-A23B-F047-9BFC-C4F6AB2A68FA}"/>
+    <hyperlink ref="E21" r:id="rId18" xr:uid="{91DC0849-A771-2B4D-8789-A3192EE6CCFF}"/>
+    <hyperlink ref="E22" r:id="rId19" xr:uid="{DCC3D403-80C5-5E49-A2EC-ECF64C647897}"/>
+    <hyperlink ref="E23" r:id="rId20" xr:uid="{EB48910F-CAED-4241-8797-59C9BA8AED93}"/>
+    <hyperlink ref="E24" r:id="rId21" xr:uid="{01534F59-E8D4-A541-B4DB-E4E6FDE7D2A7}"/>
+    <hyperlink ref="E25" r:id="rId22" xr:uid="{C2314C5D-0EE5-1244-8978-6CE7B18811FE}"/>
+    <hyperlink ref="E26" r:id="rId23" xr:uid="{6A2887EF-8B3A-0D44-A624-1078642D44C4}"/>
+    <hyperlink ref="E27" r:id="rId24" xr:uid="{9C80C4A9-D364-B447-9AAB-563D067F5FA8}"/>
+    <hyperlink ref="E28" r:id="rId25" xr:uid="{287A05EC-4791-7C4B-AFB2-EF7F9E98085F}"/>
+    <hyperlink ref="E29" r:id="rId26" xr:uid="{C39F56A0-BABE-4748-B88E-1F9C1CD5399C}"/>
+    <hyperlink ref="E30" r:id="rId27" xr:uid="{CD3500D6-E89A-4443-86B3-93668D92BD4C}"/>
+    <hyperlink ref="E31" r:id="rId28" xr:uid="{4E9031F0-8477-664F-B92D-F40965307973}"/>
+    <hyperlink ref="E32" r:id="rId29" location="tCI" xr:uid="{022F7D3A-5030-454F-969D-9C782EBCAE5D}"/>
+    <hyperlink ref="E33" r:id="rId30" location="t2CO" xr:uid="{C04AE7AD-6C42-7C4E-AA71-5AA56D31D27B}"/>
+    <hyperlink ref="E34" r:id="rId31" xr:uid="{8E40C015-C2DE-414B-AA80-95431D3A7B21}"/>
+    <hyperlink ref="E35" r:id="rId32" xr:uid="{46DA0A8F-7FE4-9242-B8D2-37F0D4DE5614}"/>
+    <hyperlink ref="E36" r:id="rId33" xr:uid="{BA2EA337-4B15-6E43-B69B-4DB9C3CC27F9}"/>
+    <hyperlink ref="E37" r:id="rId34" xr:uid="{2B632F1D-0A51-064B-A6DE-8C7259DDAAA9}"/>
+    <hyperlink ref="E38" r:id="rId35" xr:uid="{93B3DFB5-17A9-3243-BD65-EC69EA51348B}"/>
+    <hyperlink ref="E39" r:id="rId36" xr:uid="{A2C45F4E-4F2E-F547-8BC2-3DDF02AC0857}"/>
+    <hyperlink ref="E40" r:id="rId37" xr:uid="{3ABE88F8-913E-6C43-A8C5-978FBBD474BD}"/>
+    <hyperlink ref="E41" r:id="rId38" xr:uid="{9A8E5A03-D834-3D42-89F8-16C00EDC990A}"/>
+    <hyperlink ref="E42" r:id="rId39" xr:uid="{FDB9A909-7A83-1049-B137-579966521ACD}"/>
+    <hyperlink ref="E43" r:id="rId40" xr:uid="{1D912449-03D0-DC44-95AE-E65D2E7E3025}"/>
+    <hyperlink ref="E44" r:id="rId41" xr:uid="{00A22981-CD0A-3D4C-932C-B8AF0DA63F33}"/>
+    <hyperlink ref="E45" r:id="rId42" xr:uid="{2C7CDF4C-39FB-FE44-89A0-C187A8729B6B}"/>
+    <hyperlink ref="E3" r:id="rId43" xr:uid="{D5125191-C800-8B42-8AE5-37A4799280D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>